<commit_message>
Analyze result by feature rank
 For linear SVC, feature rank can be applied to absolute value of
 coefficient
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/classification_report.xlsx
+++ b/textToOps/data/processed/classification_report.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.25</v>
-      </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8461538461538461</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8148148148148148</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="E8" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -604,7 +604,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -633,13 +633,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.75</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -709,16 +709,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -747,16 +747,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -804,16 +804,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5714285714285714</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.7499999999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -823,16 +823,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6666666666666665</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.76</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="C23" t="n">
-        <v>0.76</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="D23" t="n">
-        <v>0.76</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="E23" t="n">
-        <v>0.76</v>
+        <v>0.6774193548387096</v>
       </c>
     </row>
     <row r="24">
@@ -880,16 +880,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6842403628117913</v>
+        <v>0.5166666666666666</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7563928135356707</v>
+        <v>0.5952380952380952</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6971288852241233</v>
+        <v>0.5456709956709956</v>
       </c>
       <c r="E24" t="n">
-        <v>75</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
@@ -899,16 +899,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.7484126984126984</v>
+        <v>0.5580645161290323</v>
       </c>
       <c r="C25" t="n">
-        <v>0.76</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7352403399070067</v>
+        <v>0.6041544477028348</v>
       </c>
       <c r="E25" t="n">
-        <v>75</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>